<commit_message>
Commentaires de l'api, auto evaluation partielle
</commit_message>
<xml_diff>
--- a/evaluation/evaluation.xlsx
+++ b/evaluation/evaluation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>Auto-évaluation</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Les modèles Mongoose contiennent un minimum de validations (p. ex. champs obligatoires).</t>
+  </si>
+  <si>
+    <t>1 (les tests de validité sont effectués avant l'insertion des données, dès la réception de la requête POST)</t>
   </si>
   <si>
     <t>L'implémentation de la page de garde respecte le modèle MVC d'Express.</t>
@@ -293,17 +296,17 @@
   </sheetPr>
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D52" activeCellId="0" sqref="D52"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="114.555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="117.496296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -562,13 +565,13 @@
       <c r="B27" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="0" t="n">
-        <v>0</v>
+      <c r="D27" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>1</v>
@@ -579,7 +582,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>1</v>
@@ -590,7 +593,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1</v>
@@ -617,12 +620,12 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>1</v>
@@ -633,7 +636,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>1</v>
@@ -644,7 +647,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>1</v>
@@ -652,7 +655,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>1</v>
@@ -663,7 +666,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1</v>
@@ -674,7 +677,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>1</v>
@@ -685,7 +688,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>1</v>
@@ -693,7 +696,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>1</v>
@@ -704,7 +707,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>1</v>
@@ -715,7 +718,7 @@
     </row>
     <row r="43" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>1</v>
@@ -743,12 +746,12 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>1</v>
@@ -759,7 +762,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>1</v>
@@ -770,7 +773,7 @@
     </row>
     <row r="50" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>1</v>
@@ -781,7 +784,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>1</v>
@@ -825,7 +828,7 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B58" s="1" t="n">
         <f aca="false">SUM(B7,B21,B31,B44,B52)</f>
@@ -843,7 +846,7 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B62" s="1" t="n">
         <f aca="false">B58-B52-B21</f>
@@ -852,7 +855,7 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B63" s="5" t="n">
         <f aca="false">B62/B58*5+1</f>

</xml_diff>